<commit_message>
remove b-b temp files
</commit_message>
<xml_diff>
--- a/fmri/keuka_brain_behavior_analyses/dan/MNH DAN Labels 400 Good Only 47 parcels.xlsx
+++ b/fmri/keuka_brain_behavior_analyses/dan/MNH DAN Labels 400 Good Only 47 parcels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/SCEPTIC_fMRI/dan_medusa/schaefer_400_remap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hallquist/Data_Analysis/clock_analysis/fmri/keuka_brain_behavior_analyses/dan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCDFD73-C780-0F4A-9DA4-339EEEC4342B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4EAD25-933B-3642-AD6A-DA547385765C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="229">
   <si>
     <t>roi7_200</t>
   </si>
@@ -701,6 +701,12 @@
   </si>
   <si>
     <t>network17_400_DAN</t>
+  </si>
+  <si>
+    <t>stream</t>
+  </si>
+  <si>
+    <t>visual-motion</t>
   </si>
 </sst>
 </file>
@@ -1061,22 +1067,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:W48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="13" max="14" width="17.33203125" customWidth="1"/>
+    <col min="14" max="15" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1108,43 +1114,46 @@
         <v>225</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>31</v>
       </c>
@@ -1170,43 +1179,46 @@
         <v>103</v>
       </c>
       <c r="K2" t="s">
-        <v>107</v>
+        <v>228</v>
       </c>
       <c r="L2" t="s">
         <v>107</v>
       </c>
       <c r="M2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N2" t="s">
         <v>111</v>
       </c>
       <c r="O2" t="s">
+        <v>111</v>
+      </c>
+      <c r="P2" t="s">
         <v>116</v>
-      </c>
-      <c r="P2" t="s">
-        <v>118</v>
       </c>
       <c r="Q2" t="s">
         <v>118</v>
       </c>
       <c r="R2" t="s">
+        <v>118</v>
+      </c>
+      <c r="S2" t="s">
         <v>145</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>178</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>-44</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>-42</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>-21</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1229,43 +1241,46 @@
         <v>103</v>
       </c>
       <c r="K3" t="s">
-        <v>107</v>
+        <v>228</v>
       </c>
       <c r="L3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3" t="s">
         <v>110</v>
-      </c>
-      <c r="M3" t="s">
-        <v>111</v>
       </c>
       <c r="N3" t="s">
         <v>111</v>
       </c>
       <c r="O3" t="s">
+        <v>111</v>
+      </c>
+      <c r="P3" t="s">
         <v>116</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>120</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>21</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>147</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>180</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>-48</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>-55</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>-15</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1288,43 +1303,46 @@
         <v>103</v>
       </c>
       <c r="K4" t="s">
-        <v>107</v>
+        <v>228</v>
       </c>
       <c r="L4" t="s">
+        <v>107</v>
+      </c>
+      <c r="M4" t="s">
         <v>110</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>111</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>112</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>116</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>119</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>21</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>146</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>179</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>-54</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>-62</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1353,43 +1371,46 @@
         <v>103</v>
       </c>
       <c r="K5" t="s">
-        <v>107</v>
+        <v>228</v>
       </c>
       <c r="L5" t="s">
+        <v>107</v>
+      </c>
+      <c r="M5" t="s">
         <v>110</v>
-      </c>
-      <c r="M5" t="s">
-        <v>111</v>
       </c>
       <c r="N5" t="s">
         <v>111</v>
       </c>
       <c r="O5" t="s">
+        <v>111</v>
+      </c>
+      <c r="P5" t="s">
         <v>116</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>140</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>23</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>167</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>200</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>-46</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>-68</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>14</v>
       </c>
@@ -1411,44 +1432,44 @@
       <c r="J6" t="s">
         <v>106</v>
       </c>
-      <c r="K6" t="s">
-        <v>107</v>
-      </c>
       <c r="L6" t="s">
+        <v>107</v>
+      </c>
+      <c r="M6" t="s">
         <v>110</v>
-      </c>
-      <c r="M6" t="s">
-        <v>111</v>
       </c>
       <c r="N6" t="s">
         <v>111</v>
       </c>
       <c r="O6" t="s">
+        <v>111</v>
+      </c>
+      <c r="P6" t="s">
         <v>116</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>132</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>28</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>159</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>192</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>-27</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>-70</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>34</v>
       </c>
@@ -1476,44 +1497,44 @@
       <c r="J7" t="s">
         <v>105</v>
       </c>
-      <c r="K7" t="s">
-        <v>107</v>
-      </c>
       <c r="L7" t="s">
         <v>107</v>
       </c>
       <c r="M7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N7" t="s">
         <v>113</v>
       </c>
       <c r="O7" t="s">
+        <v>113</v>
+      </c>
+      <c r="P7" t="s">
         <v>116</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>136</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>140</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>163</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>196</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>-53</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>-31</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>33</v>
       </c>
@@ -1541,44 +1562,44 @@
       <c r="J8" t="s">
         <v>106</v>
       </c>
-      <c r="K8" t="s">
-        <v>107</v>
-      </c>
       <c r="L8" t="s">
         <v>107</v>
       </c>
       <c r="M8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N8" t="s">
         <v>111</v>
       </c>
       <c r="O8" t="s">
+        <v>111</v>
+      </c>
+      <c r="P8" t="s">
         <v>116</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>131</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>119</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>158</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>191</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>-24</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>-64</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>23</v>
       </c>
@@ -1603,44 +1624,44 @@
       <c r="J9" t="s">
         <v>105</v>
       </c>
-      <c r="K9" t="s">
-        <v>107</v>
-      </c>
       <c r="L9" t="s">
+        <v>107</v>
+      </c>
+      <c r="M9" t="s">
         <v>109</v>
       </c>
-      <c r="M9" t="s">
-        <v>113</v>
-      </c>
       <c r="N9" t="s">
         <v>113</v>
       </c>
       <c r="O9" t="s">
+        <v>113</v>
+      </c>
+      <c r="P9" t="s">
         <v>116</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>123</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>24</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>150</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>183</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>-43</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>-30</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>36</v>
       </c>
@@ -1665,44 +1686,44 @@
       <c r="J10" t="s">
         <v>106</v>
       </c>
-      <c r="K10" t="s">
-        <v>107</v>
-      </c>
       <c r="L10" t="s">
         <v>107</v>
       </c>
       <c r="M10" t="s">
+        <v>107</v>
+      </c>
+      <c r="N10" t="s">
         <v>111</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>112</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>116</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>138</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>136</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>165</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>198</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>-33</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>-46</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>33</v>
       </c>
@@ -1727,44 +1748,44 @@
       <c r="J11" t="s">
         <v>106</v>
       </c>
-      <c r="K11" t="s">
-        <v>107</v>
-      </c>
       <c r="L11" t="s">
         <v>107</v>
       </c>
       <c r="M11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N11" t="s">
         <v>111</v>
       </c>
       <c r="O11" t="s">
+        <v>111</v>
+      </c>
+      <c r="P11" t="s">
         <v>116</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>130</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>119</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>157</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>190</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>-28</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>-58</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>25</v>
       </c>
@@ -1789,44 +1810,44 @@
       <c r="J12" t="s">
         <v>105</v>
       </c>
-      <c r="K12" t="s">
-        <v>107</v>
-      </c>
       <c r="L12" t="s">
+        <v>107</v>
+      </c>
+      <c r="M12" t="s">
         <v>109</v>
       </c>
-      <c r="M12" t="s">
-        <v>113</v>
-      </c>
       <c r="N12" t="s">
         <v>113</v>
       </c>
       <c r="O12" t="s">
+        <v>113</v>
+      </c>
+      <c r="P12" t="s">
         <v>116</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>124</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>26</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>151</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>184</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>-36</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>-37</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>25</v>
       </c>
@@ -1851,44 +1872,44 @@
       <c r="J13" t="s">
         <v>106</v>
       </c>
-      <c r="K13" t="s">
-        <v>107</v>
-      </c>
       <c r="L13" t="s">
+        <v>107</v>
+      </c>
+      <c r="M13" t="s">
         <v>109</v>
-      </c>
-      <c r="M13" t="s">
-        <v>111</v>
       </c>
       <c r="N13" t="s">
         <v>111</v>
       </c>
       <c r="O13" t="s">
+        <v>111</v>
+      </c>
+      <c r="P13" t="s">
         <v>116</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>139</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>26</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>166</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>199</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>-35</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>-50</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>37</v>
       </c>
@@ -1916,44 +1937,44 @@
       <c r="J14" t="s">
         <v>106</v>
       </c>
-      <c r="K14" t="s">
-        <v>107</v>
-      </c>
       <c r="L14" t="s">
         <v>107</v>
       </c>
       <c r="M14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N14" t="s">
         <v>111</v>
       </c>
       <c r="O14" t="s">
+        <v>111</v>
+      </c>
+      <c r="P14" t="s">
         <v>116</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>133</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>131</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>160</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>193</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>-15</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>-69</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>37</v>
       </c>
@@ -1981,44 +2002,44 @@
       <c r="J15" t="s">
         <v>106</v>
       </c>
-      <c r="K15" t="s">
-        <v>107</v>
-      </c>
       <c r="L15" t="s">
         <v>107</v>
       </c>
       <c r="M15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N15" t="s">
         <v>111</v>
       </c>
       <c r="O15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P15" t="s">
         <v>116</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>129</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>131</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>156</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>189</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>-27</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>-58</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>39</v>
       </c>
@@ -2043,44 +2064,44 @@
       <c r="J16" t="s">
         <v>105</v>
       </c>
-      <c r="K16" t="s">
-        <v>107</v>
-      </c>
       <c r="L16" t="s">
         <v>107</v>
       </c>
       <c r="M16" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N16" t="s">
         <v>113</v>
       </c>
       <c r="O16" t="s">
+        <v>113</v>
+      </c>
+      <c r="P16" t="s">
         <v>116</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>134</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>138</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>161</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>194</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>-7</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>-57</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>25</v>
       </c>
@@ -2105,44 +2126,44 @@
       <c r="J17" t="s">
         <v>105</v>
       </c>
-      <c r="K17" t="s">
-        <v>107</v>
-      </c>
       <c r="L17" t="s">
+        <v>107</v>
+      </c>
+      <c r="M17" t="s">
         <v>109</v>
       </c>
-      <c r="M17" t="s">
-        <v>113</v>
-      </c>
       <c r="N17" t="s">
         <v>113</v>
       </c>
       <c r="O17" t="s">
+        <v>113</v>
+      </c>
+      <c r="P17" t="s">
         <v>116</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>122</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>26</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>149</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>182</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>-20</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>-54</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>21</v>
       </c>
@@ -2164,44 +2185,44 @@
       <c r="J18" t="s">
         <v>104</v>
       </c>
-      <c r="K18" t="s">
-        <v>107</v>
-      </c>
       <c r="L18" t="s">
+        <v>107</v>
+      </c>
+      <c r="M18" t="s">
         <v>109</v>
       </c>
-      <c r="M18" t="s">
-        <v>113</v>
-      </c>
       <c r="N18" t="s">
         <v>113</v>
       </c>
       <c r="O18" t="s">
+        <v>113</v>
+      </c>
+      <c r="P18" t="s">
         <v>116</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>127</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>22</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>154</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>187</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>-40</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>-4</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>41</v>
       </c>
@@ -2226,44 +2247,44 @@
       <c r="J19" t="s">
         <v>104</v>
       </c>
-      <c r="K19" t="s">
-        <v>107</v>
-      </c>
       <c r="L19" t="s">
         <v>107</v>
       </c>
       <c r="M19" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N19" t="s">
         <v>113</v>
       </c>
       <c r="O19" t="s">
+        <v>113</v>
+      </c>
+      <c r="P19" t="s">
         <v>116</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>126</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>127</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>153</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>186</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>-26</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>-2</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>41</v>
       </c>
@@ -2288,44 +2309,44 @@
       <c r="J20" t="s">
         <v>104</v>
       </c>
-      <c r="K20" t="s">
-        <v>107</v>
-      </c>
       <c r="L20" t="s">
         <v>107</v>
       </c>
       <c r="M20" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N20" t="s">
         <v>113</v>
       </c>
       <c r="O20" t="s">
+        <v>113</v>
+      </c>
+      <c r="P20" t="s">
         <v>116</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>128</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>127</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>155</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>188</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>-30</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>-9</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>28</v>
       </c>
@@ -2350,44 +2371,44 @@
       <c r="J21" t="s">
         <v>104</v>
       </c>
-      <c r="K21" t="s">
-        <v>107</v>
-      </c>
       <c r="L21" t="s">
+        <v>107</v>
+      </c>
+      <c r="M21" t="s">
         <v>109</v>
       </c>
-      <c r="M21" t="s">
-        <v>113</v>
-      </c>
       <c r="N21" t="s">
+        <v>113</v>
+      </c>
+      <c r="O21" t="s">
         <v>112</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>116</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>121</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>28</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>148</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>181</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>-21</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>3</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>43</v>
       </c>
@@ -2415,44 +2436,44 @@
       <c r="J22" t="s">
         <v>104</v>
       </c>
-      <c r="K22" t="s">
-        <v>107</v>
-      </c>
       <c r="L22" t="s">
         <v>107</v>
       </c>
       <c r="M22" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N22" t="s">
+        <v>113</v>
+      </c>
+      <c r="O22" t="s">
         <v>112</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>116</v>
-      </c>
-      <c r="P22" t="s">
-        <v>125</v>
       </c>
       <c r="Q22" t="s">
         <v>125</v>
       </c>
       <c r="R22" t="s">
+        <v>125</v>
+      </c>
+      <c r="S22" t="s">
         <v>152</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>185</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>-48</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>6</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2474,44 +2495,44 @@
       <c r="J23" t="s">
         <v>104</v>
       </c>
-      <c r="K23" t="s">
-        <v>107</v>
-      </c>
       <c r="L23" t="s">
+        <v>107</v>
+      </c>
+      <c r="M23" t="s">
         <v>109</v>
       </c>
-      <c r="M23" t="s">
-        <v>113</v>
-      </c>
       <c r="N23" t="s">
         <v>113</v>
       </c>
       <c r="O23" t="s">
+        <v>113</v>
+      </c>
+      <c r="P23" t="s">
         <v>116</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>137</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>22</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>164</v>
       </c>
-      <c r="S23" t="s">
+      <c r="T23" t="s">
         <v>197</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>-49</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>1</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>39</v>
       </c>
@@ -2539,44 +2560,44 @@
       <c r="J24" t="s">
         <v>105</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>108</v>
       </c>
-      <c r="L24" t="s">
-        <v>107</v>
-      </c>
       <c r="M24" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N24" t="s">
+        <v>113</v>
+      </c>
+      <c r="O24" t="s">
         <v>114</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>116</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>135</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>138</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>162</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>195</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>-4</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <v>-62</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>147</v>
       </c>
@@ -2604,44 +2625,44 @@
       <c r="J25" t="s">
         <v>104</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>109</v>
       </c>
-      <c r="L25" t="s">
-        <v>107</v>
-      </c>
       <c r="M25" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N25" t="s">
+        <v>113</v>
+      </c>
+      <c r="O25" t="s">
         <v>115</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>117</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>29</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>125</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>170</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>210</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>59</v>
       </c>
-      <c r="U25">
+      <c r="V25">
         <v>6</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>101</v>
       </c>
@@ -2664,43 +2685,46 @@
         <v>103</v>
       </c>
       <c r="K26" t="s">
-        <v>107</v>
+        <v>228</v>
       </c>
       <c r="L26" t="s">
+        <v>107</v>
+      </c>
+      <c r="M26" t="s">
         <v>110</v>
-      </c>
-      <c r="M26" t="s">
-        <v>111</v>
       </c>
       <c r="N26" t="s">
         <v>111</v>
       </c>
       <c r="O26" t="s">
+        <v>111</v>
+      </c>
+      <c r="P26" t="s">
         <v>117</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>118</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>20</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>168</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>201</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <v>48</v>
       </c>
-      <c r="U26">
+      <c r="V26">
         <v>-51</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>-17</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>135</v>
       </c>
@@ -2729,43 +2753,46 @@
         <v>103</v>
       </c>
       <c r="K27" t="s">
-        <v>107</v>
+        <v>228</v>
       </c>
       <c r="L27" t="s">
         <v>107</v>
       </c>
       <c r="M27" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N27" t="s">
         <v>113</v>
       </c>
       <c r="O27" t="s">
+        <v>113</v>
+      </c>
+      <c r="P27" t="s">
         <v>117</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>120</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>118</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>145</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>203</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>58</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>-56</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>136</v>
       </c>
@@ -2791,43 +2818,46 @@
         <v>103</v>
       </c>
       <c r="K28" t="s">
-        <v>107</v>
+        <v>228</v>
       </c>
       <c r="L28" t="s">
         <v>107</v>
       </c>
       <c r="M28" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N28" t="s">
         <v>111</v>
       </c>
       <c r="O28" t="s">
+        <v>111</v>
+      </c>
+      <c r="P28" t="s">
         <v>117</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>119</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
         <v>120</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>169</v>
       </c>
-      <c r="S28" t="s">
+      <c r="T28" t="s">
         <v>202</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>52</v>
       </c>
-      <c r="U28">
+      <c r="V28">
         <v>-57</v>
       </c>
-      <c r="V28">
+      <c r="W28">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>115</v>
       </c>
@@ -2855,44 +2885,44 @@
       <c r="J29" t="s">
         <v>106</v>
       </c>
-      <c r="K29" t="s">
-        <v>107</v>
-      </c>
       <c r="L29" t="s">
+        <v>107</v>
+      </c>
+      <c r="M29" t="s">
         <v>110</v>
-      </c>
-      <c r="M29" t="s">
-        <v>111</v>
       </c>
       <c r="N29" t="s">
         <v>111</v>
       </c>
       <c r="O29" t="s">
+        <v>111</v>
+      </c>
+      <c r="P29" t="s">
         <v>117</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>132</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>29</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>172</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>215</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>31</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <v>-67</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>137</v>
       </c>
@@ -2917,44 +2947,44 @@
       <c r="J30" t="s">
         <v>105</v>
       </c>
-      <c r="K30" t="s">
-        <v>107</v>
-      </c>
       <c r="L30" t="s">
         <v>107</v>
       </c>
       <c r="M30" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N30" t="s">
         <v>113</v>
       </c>
       <c r="O30" t="s">
+        <v>113</v>
+      </c>
+      <c r="P30" t="s">
         <v>117</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>136</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>119</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>176</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>222</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>55</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <v>-25</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>114</v>
       </c>
@@ -2976,44 +3006,44 @@
       <c r="J31" t="s">
         <v>106</v>
       </c>
-      <c r="K31" t="s">
-        <v>107</v>
-      </c>
       <c r="L31" t="s">
+        <v>107</v>
+      </c>
+      <c r="M31" t="s">
         <v>110</v>
-      </c>
-      <c r="M31" t="s">
-        <v>111</v>
       </c>
       <c r="N31" t="s">
         <v>111</v>
       </c>
       <c r="O31" t="s">
+        <v>111</v>
+      </c>
+      <c r="P31" t="s">
         <v>117</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>131</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>28</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>158</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>218</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <v>17</v>
       </c>
-      <c r="U31">
+      <c r="V31">
         <v>-76</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>138</v>
       </c>
@@ -3038,44 +3068,44 @@
       <c r="J32" t="s">
         <v>105</v>
       </c>
-      <c r="K32" t="s">
-        <v>107</v>
-      </c>
       <c r="L32" t="s">
         <v>107</v>
       </c>
       <c r="M32" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N32" t="s">
         <v>113</v>
       </c>
       <c r="O32" t="s">
+        <v>113</v>
+      </c>
+      <c r="P32" t="s">
         <v>117</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>123</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>140</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>163</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>209</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>38</v>
       </c>
-      <c r="U32">
+      <c r="V32">
         <v>-39</v>
       </c>
-      <c r="V32">
+      <c r="W32">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>124</v>
       </c>
@@ -3097,44 +3127,44 @@
       <c r="J33" t="s">
         <v>105</v>
       </c>
-      <c r="K33" t="s">
-        <v>107</v>
-      </c>
       <c r="L33" t="s">
+        <v>107</v>
+      </c>
+      <c r="M33" t="s">
         <v>109</v>
       </c>
-      <c r="M33" t="s">
-        <v>113</v>
-      </c>
       <c r="N33" t="s">
         <v>113</v>
       </c>
       <c r="O33" t="s">
+        <v>113</v>
+      </c>
+      <c r="P33" t="s">
         <v>117</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>138</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="R33" t="s">
         <v>24</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>150</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>208</v>
       </c>
-      <c r="T33">
+      <c r="U33">
         <v>43</v>
       </c>
-      <c r="U33">
+      <c r="V33">
         <v>-29</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>142</v>
       </c>
@@ -3159,44 +3189,44 @@
       <c r="J34" t="s">
         <v>106</v>
       </c>
-      <c r="K34" t="s">
-        <v>107</v>
-      </c>
       <c r="L34" t="s">
         <v>107</v>
       </c>
       <c r="M34" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N34" t="s">
         <v>111</v>
       </c>
       <c r="O34" t="s">
+        <v>111</v>
+      </c>
+      <c r="P34" t="s">
         <v>117</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>130</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="R34" t="s">
         <v>123</v>
       </c>
-      <c r="R34" t="s">
+      <c r="S34" t="s">
         <v>157</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>216</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <v>28</v>
       </c>
-      <c r="U34">
+      <c r="V34">
         <v>-61</v>
       </c>
-      <c r="V34">
+      <c r="W34">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>138</v>
       </c>
@@ -3221,44 +3251,44 @@
       <c r="J35" t="s">
         <v>106</v>
       </c>
-      <c r="K35" t="s">
-        <v>107</v>
-      </c>
       <c r="L35" t="s">
         <v>107</v>
       </c>
       <c r="M35" t="s">
+        <v>107</v>
+      </c>
+      <c r="N35" t="s">
         <v>111</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>112</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>117</v>
       </c>
-      <c r="P35" t="s">
+      <c r="Q35" t="s">
         <v>124</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="R35" t="s">
         <v>140</v>
       </c>
-      <c r="R35" t="s">
+      <c r="S35" t="s">
         <v>177</v>
       </c>
-      <c r="S35" t="s">
+      <c r="T35" t="s">
         <v>223</v>
       </c>
-      <c r="T35">
+      <c r="U35">
         <v>32</v>
       </c>
-      <c r="U35">
+      <c r="V35">
         <v>-46</v>
       </c>
-      <c r="V35">
+      <c r="W35">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>115</v>
       </c>
@@ -3280,44 +3310,44 @@
       <c r="J36" t="s">
         <v>106</v>
       </c>
-      <c r="K36" t="s">
-        <v>107</v>
-      </c>
       <c r="L36" t="s">
+        <v>107</v>
+      </c>
+      <c r="M36" t="s">
         <v>110</v>
-      </c>
-      <c r="M36" t="s">
-        <v>111</v>
       </c>
       <c r="N36" t="s">
         <v>111</v>
       </c>
       <c r="O36" t="s">
+        <v>111</v>
+      </c>
+      <c r="P36" t="s">
         <v>117</v>
       </c>
-      <c r="P36" t="s">
+      <c r="Q36" t="s">
         <v>139</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="R36" t="s">
         <v>29</v>
       </c>
-      <c r="R36" t="s">
+      <c r="S36" t="s">
         <v>166</v>
       </c>
-      <c r="S36" t="s">
+      <c r="T36" t="s">
         <v>217</v>
       </c>
-      <c r="T36">
+      <c r="U36">
         <v>20</v>
       </c>
-      <c r="U36">
+      <c r="V36">
         <v>-68</v>
       </c>
-      <c r="V36">
+      <c r="W36">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>124</v>
       </c>
@@ -3342,44 +3372,44 @@
       <c r="J37" t="s">
         <v>105</v>
       </c>
-      <c r="K37" t="s">
-        <v>107</v>
-      </c>
       <c r="L37" t="s">
+        <v>107</v>
+      </c>
+      <c r="M37" t="s">
         <v>109</v>
       </c>
-      <c r="M37" t="s">
-        <v>113</v>
-      </c>
       <c r="N37" t="s">
         <v>113</v>
       </c>
       <c r="O37" t="s">
+        <v>113</v>
+      </c>
+      <c r="P37" t="s">
         <v>117</v>
       </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>133</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="R37" t="s">
         <v>24</v>
       </c>
-      <c r="R37" t="s">
+      <c r="S37" t="s">
         <v>151</v>
       </c>
-      <c r="S37" t="s">
+      <c r="T37" t="s">
         <v>207</v>
       </c>
-      <c r="T37">
+      <c r="U37">
         <v>38</v>
       </c>
-      <c r="U37">
+      <c r="V37">
         <v>-38</v>
       </c>
-      <c r="V37">
+      <c r="W37">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>128</v>
       </c>
@@ -3401,44 +3431,44 @@
       <c r="J38" t="s">
         <v>106</v>
       </c>
-      <c r="K38" t="s">
-        <v>107</v>
-      </c>
       <c r="L38" t="s">
+        <v>107</v>
+      </c>
+      <c r="M38" t="s">
         <v>109</v>
-      </c>
-      <c r="M38" t="s">
-        <v>111</v>
       </c>
       <c r="N38" t="s">
         <v>111</v>
       </c>
       <c r="O38" t="s">
+        <v>111</v>
+      </c>
+      <c r="P38" t="s">
         <v>117</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>129</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>27</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>160</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>224</v>
       </c>
-      <c r="T38">
+      <c r="U38">
         <v>33</v>
       </c>
-      <c r="U38">
+      <c r="V38">
         <v>-52</v>
       </c>
-      <c r="V38">
+      <c r="W38">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>140</v>
       </c>
@@ -3463,44 +3493,44 @@
       <c r="J39" t="s">
         <v>106</v>
       </c>
-      <c r="K39" t="s">
-        <v>107</v>
-      </c>
       <c r="L39" t="s">
         <v>107</v>
       </c>
       <c r="M39" t="s">
+        <v>107</v>
+      </c>
+      <c r="N39" t="s">
         <v>111</v>
       </c>
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>114</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>117</v>
       </c>
-      <c r="P39" t="s">
+      <c r="Q39" t="s">
         <v>134</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="R39" t="s">
         <v>136</v>
       </c>
-      <c r="R39" t="s">
+      <c r="S39" t="s">
         <v>173</v>
       </c>
-      <c r="S39" t="s">
+      <c r="T39" t="s">
         <v>219</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <v>7</v>
       </c>
-      <c r="U39">
+      <c r="V39">
         <v>-70</v>
       </c>
-      <c r="V39">
+      <c r="W39">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>142</v>
       </c>
@@ -3525,44 +3555,44 @@
       <c r="J40" t="s">
         <v>106</v>
       </c>
-      <c r="K40" t="s">
-        <v>107</v>
-      </c>
       <c r="L40" t="s">
         <v>107</v>
       </c>
       <c r="M40" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N40" t="s">
         <v>111</v>
       </c>
       <c r="O40" t="s">
+        <v>111</v>
+      </c>
+      <c r="P40" t="s">
         <v>117</v>
       </c>
-      <c r="P40" t="s">
+      <c r="Q40" t="s">
         <v>122</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="R40" t="s">
         <v>123</v>
       </c>
-      <c r="R40" t="s">
+      <c r="S40" t="s">
         <v>156</v>
       </c>
-      <c r="S40" t="s">
+      <c r="T40" t="s">
         <v>214</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <v>26</v>
       </c>
-      <c r="U40">
+      <c r="V40">
         <v>-58</v>
       </c>
-      <c r="V40">
+      <c r="W40">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>143</v>
       </c>
@@ -3587,44 +3617,44 @@
       <c r="J41" t="s">
         <v>105</v>
       </c>
-      <c r="K41" t="s">
-        <v>107</v>
-      </c>
       <c r="L41" t="s">
         <v>107</v>
       </c>
       <c r="M41" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N41" t="s">
         <v>113</v>
       </c>
       <c r="O41" t="s">
+        <v>113</v>
+      </c>
+      <c r="P41" t="s">
         <v>117</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
         <v>144</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="R41" t="s">
         <v>138</v>
       </c>
-      <c r="R41" t="s">
+      <c r="S41" t="s">
         <v>175</v>
       </c>
-      <c r="S41" t="s">
+      <c r="T41" t="s">
         <v>221</v>
       </c>
-      <c r="T41">
+      <c r="U41">
         <v>7</v>
       </c>
-      <c r="U41">
+      <c r="V41">
         <v>-53</v>
       </c>
-      <c r="V41">
+      <c r="W41">
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>140</v>
       </c>
@@ -3649,44 +3679,44 @@
       <c r="J42" t="s">
         <v>106</v>
       </c>
-      <c r="K42" t="s">
-        <v>107</v>
-      </c>
       <c r="L42" t="s">
         <v>107</v>
       </c>
       <c r="M42" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N42" t="s">
         <v>111</v>
       </c>
       <c r="O42" t="s">
+        <v>111</v>
+      </c>
+      <c r="P42" t="s">
         <v>117</v>
       </c>
-      <c r="P42" t="s">
+      <c r="Q42" t="s">
         <v>143</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="R42" t="s">
         <v>136</v>
       </c>
-      <c r="R42" t="s">
+      <c r="S42" t="s">
         <v>174</v>
       </c>
-      <c r="S42" t="s">
+      <c r="T42" t="s">
         <v>220</v>
       </c>
-      <c r="T42">
+      <c r="U42">
         <v>13</v>
       </c>
-      <c r="U42">
+      <c r="V42">
         <v>-63</v>
       </c>
-      <c r="V42">
+      <c r="W42">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>128</v>
       </c>
@@ -3708,44 +3738,44 @@
       <c r="J43" t="s">
         <v>105</v>
       </c>
-      <c r="K43" t="s">
-        <v>107</v>
-      </c>
       <c r="L43" t="s">
+        <v>107</v>
+      </c>
+      <c r="M43" t="s">
         <v>109</v>
       </c>
-      <c r="M43" t="s">
-        <v>113</v>
-      </c>
       <c r="N43" t="s">
         <v>113</v>
       </c>
       <c r="O43" t="s">
+        <v>113</v>
+      </c>
+      <c r="P43" t="s">
         <v>117</v>
       </c>
-      <c r="P43" t="s">
+      <c r="Q43" t="s">
         <v>142</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="R43" t="s">
         <v>27</v>
       </c>
-      <c r="R43" t="s">
+      <c r="S43" t="s">
         <v>161</v>
       </c>
-      <c r="S43" t="s">
+      <c r="T43" t="s">
         <v>206</v>
       </c>
-      <c r="T43">
+      <c r="U43">
         <v>25</v>
       </c>
-      <c r="U43">
+      <c r="V43">
         <v>-51</v>
       </c>
-      <c r="V43">
+      <c r="W43">
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>125</v>
       </c>
@@ -3767,44 +3797,44 @@
       <c r="J44" t="s">
         <v>104</v>
       </c>
-      <c r="K44" t="s">
-        <v>107</v>
-      </c>
       <c r="L44" t="s">
+        <v>107</v>
+      </c>
+      <c r="M44" t="s">
         <v>109</v>
       </c>
-      <c r="M44" t="s">
-        <v>113</v>
-      </c>
       <c r="N44" t="s">
         <v>113</v>
       </c>
       <c r="O44" t="s">
+        <v>113</v>
+      </c>
+      <c r="P44" t="s">
         <v>117</v>
       </c>
-      <c r="P44" t="s">
+      <c r="Q44" t="s">
         <v>127</v>
       </c>
-      <c r="Q44" t="s">
+      <c r="R44" t="s">
         <v>25</v>
       </c>
-      <c r="R44" t="s">
+      <c r="S44" t="s">
         <v>154</v>
       </c>
-      <c r="S44" t="s">
+      <c r="T44" t="s">
         <v>213</v>
       </c>
-      <c r="T44">
+      <c r="U44">
         <v>39</v>
       </c>
-      <c r="U44">
+      <c r="V44">
         <v>-3</v>
       </c>
-      <c r="V44">
+      <c r="W44">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>131</v>
       </c>
@@ -3826,44 +3856,44 @@
       <c r="J45" t="s">
         <v>104</v>
       </c>
-      <c r="K45" t="s">
-        <v>107</v>
-      </c>
       <c r="L45" t="s">
+        <v>107</v>
+      </c>
+      <c r="M45" t="s">
         <v>109</v>
       </c>
-      <c r="M45" t="s">
-        <v>113</v>
-      </c>
       <c r="N45" t="s">
         <v>113</v>
       </c>
       <c r="O45" t="s">
+        <v>113</v>
+      </c>
+      <c r="P45" t="s">
         <v>117</v>
       </c>
-      <c r="P45" t="s">
+      <c r="Q45" t="s">
         <v>126</v>
       </c>
-      <c r="Q45" t="s">
+      <c r="R45" t="s">
         <v>30</v>
       </c>
-      <c r="R45" t="s">
+      <c r="S45" t="s">
         <v>153</v>
       </c>
-      <c r="S45" t="s">
+      <c r="T45" t="s">
         <v>212</v>
       </c>
-      <c r="T45">
+      <c r="U45">
         <v>27</v>
       </c>
-      <c r="U45">
+      <c r="V45">
         <v>-4</v>
       </c>
-      <c r="V45">
+      <c r="W45">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>131</v>
       </c>
@@ -3891,44 +3921,44 @@
       <c r="J46" t="s">
         <v>104</v>
       </c>
-      <c r="K46" t="s">
-        <v>107</v>
-      </c>
       <c r="L46" t="s">
+        <v>107</v>
+      </c>
+      <c r="M46" t="s">
         <v>109</v>
       </c>
-      <c r="M46" t="s">
-        <v>113</v>
-      </c>
       <c r="N46" t="s">
         <v>113</v>
       </c>
       <c r="O46" t="s">
+        <v>113</v>
+      </c>
+      <c r="P46" t="s">
         <v>117</v>
       </c>
-      <c r="P46" t="s">
+      <c r="Q46" t="s">
         <v>128</v>
       </c>
-      <c r="Q46" t="s">
+      <c r="R46" t="s">
         <v>30</v>
       </c>
-      <c r="R46" t="s">
+      <c r="S46" t="s">
         <v>155</v>
       </c>
-      <c r="S46" t="s">
+      <c r="T46" t="s">
         <v>204</v>
       </c>
-      <c r="T46">
+      <c r="U46">
         <v>24</v>
       </c>
-      <c r="U46">
+      <c r="V46">
         <v>-4</v>
       </c>
-      <c r="V46">
+      <c r="W46">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>147</v>
       </c>
@@ -3953,44 +3983,44 @@
       <c r="J47" t="s">
         <v>104</v>
       </c>
-      <c r="K47" t="s">
-        <v>107</v>
-      </c>
       <c r="L47" t="s">
         <v>107</v>
       </c>
       <c r="M47" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N47" t="s">
+        <v>113</v>
+      </c>
+      <c r="O47" t="s">
         <v>112</v>
       </c>
-      <c r="O47" t="s">
+      <c r="P47" t="s">
         <v>117</v>
-      </c>
-      <c r="P47" t="s">
-        <v>125</v>
       </c>
       <c r="Q47" t="s">
         <v>125</v>
       </c>
       <c r="R47" t="s">
+        <v>125</v>
+      </c>
+      <c r="S47" t="s">
         <v>171</v>
       </c>
-      <c r="S47" t="s">
+      <c r="T47" t="s">
         <v>211</v>
       </c>
-      <c r="T47">
+      <c r="U47">
         <v>48</v>
       </c>
-      <c r="U47">
+      <c r="V47">
         <v>8</v>
       </c>
-      <c r="V47">
+      <c r="W47">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>146</v>
       </c>
@@ -4021,45 +4051,45 @@
       <c r="J48" t="s">
         <v>104</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>108</v>
       </c>
-      <c r="L48" t="s">
-        <v>107</v>
-      </c>
       <c r="M48" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N48" t="s">
+        <v>113</v>
+      </c>
+      <c r="O48" t="s">
         <v>112</v>
       </c>
-      <c r="O48" t="s">
+      <c r="P48" t="s">
         <v>117</v>
       </c>
-      <c r="P48" t="s">
+      <c r="Q48" t="s">
         <v>141</v>
       </c>
-      <c r="Q48" t="s">
+      <c r="R48" t="s">
         <v>126</v>
       </c>
-      <c r="R48" t="s">
+      <c r="S48" t="s">
         <v>148</v>
       </c>
-      <c r="S48" t="s">
+      <c r="T48" t="s">
         <v>205</v>
       </c>
-      <c r="T48">
+      <c r="U48">
         <v>24</v>
       </c>
-      <c r="U48">
+      <c r="V48">
         <v>8</v>
       </c>
-      <c r="V48">
+      <c r="W48">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V48">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W48">
     <sortCondition ref="B2:B48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated DAN 47 with PMv labels
</commit_message>
<xml_diff>
--- a/fmri/keuka_brain_behavior_analyses/dan/MNH DAN Labels 400 Good Only 47 parcels.xlsx
+++ b/fmri/keuka_brain_behavior_analyses/dan/MNH DAN Labels 400 Good Only 47 parcels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hallquist/Data_Analysis/clock_analysis/fmri/keuka_brain_behavior_analyses/dan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4EAD25-933B-3642-AD6A-DA547385765C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAAAEF2-A6BC-F64B-B2DE-47409756E532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="267">
   <si>
     <t>roi7_200</t>
   </si>
@@ -211,9 +211,6 @@
     <t>L_Pcu_7P</t>
   </si>
   <si>
-    <t>L_PMv</t>
-  </si>
-  <si>
     <t>L_pVIP_Inferior</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
     <t>Tiny</t>
   </si>
   <si>
-    <t>PMv may be a more neutral and better label</t>
-  </si>
-  <si>
     <t>captures LIP voxels that sit squarely in IPS; extend inferiorly</t>
   </si>
   <si>
@@ -707,6 +701,126 @@
   </si>
   <si>
     <t>visual-motion</t>
+  </si>
+  <si>
+    <t>gg_label</t>
+  </si>
+  <si>
+    <t>Anterior MT/FST</t>
+  </si>
+  <si>
+    <t>Posterior MT/FST</t>
+  </si>
+  <si>
+    <t>MT/MST</t>
+  </si>
+  <si>
+    <t>TPJ</t>
+  </si>
+  <si>
+    <t>LIPp</t>
+  </si>
+  <si>
+    <t>Inferior LIPp</t>
+  </si>
+  <si>
+    <t>PFt</t>
+  </si>
+  <si>
+    <t>Anterior AIPa</t>
+  </si>
+  <si>
+    <t>Inferior pVIP</t>
+  </si>
+  <si>
+    <t>Posterior LIPa</t>
+  </si>
+  <si>
+    <t>Posterior AIPa</t>
+  </si>
+  <si>
+    <t>Superior pVIP</t>
+  </si>
+  <si>
+    <t>MIP</t>
+  </si>
+  <si>
+    <t>LIPa</t>
+  </si>
+  <si>
+    <t>Pcu/7A</t>
+  </si>
+  <si>
+    <t>7A/5L</t>
+  </si>
+  <si>
+    <t>Lateral FEF</t>
+  </si>
+  <si>
+    <t>FEF/6A</t>
+  </si>
+  <si>
+    <t>Medial FEF</t>
+  </si>
+  <si>
+    <t>PMd/6A</t>
+  </si>
+  <si>
+    <t>Pcu/7P</t>
+  </si>
+  <si>
+    <t>MT/FST</t>
+  </si>
+  <si>
+    <t>Inferior MT/MST</t>
+  </si>
+  <si>
+    <t>Anterior MT/MST</t>
+  </si>
+  <si>
+    <t>MIP/LIPp</t>
+  </si>
+  <si>
+    <t>Ventral LIPp</t>
+  </si>
+  <si>
+    <t>Lateral MIP</t>
+  </si>
+  <si>
+    <t>AIP</t>
+  </si>
+  <si>
+    <t>Medial MIP</t>
+  </si>
+  <si>
+    <t>Dorsal LIPp</t>
+  </si>
+  <si>
+    <t>Pcu/7A/5M</t>
+  </si>
+  <si>
+    <t>Pcu/7A/5L</t>
+  </si>
+  <si>
+    <t>Anterior PMd/6A</t>
+  </si>
+  <si>
+    <t>Initially called "L_PMv"</t>
+  </si>
+  <si>
+    <t>L_PMv1</t>
+  </si>
+  <si>
+    <t>PMv may be a more neutral and better label; Initially called L_F5_Broca</t>
+  </si>
+  <si>
+    <t>L_PMv2</t>
+  </si>
+  <si>
+    <t>PMv dorsal</t>
+  </si>
+  <si>
+    <t>PMv ventral</t>
   </si>
 </sst>
 </file>
@@ -1067,22 +1181,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W48"/>
+  <dimension ref="A1:X48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
+      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="14" max="15" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="34" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+    <col min="15" max="16" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1105,55 +1220,58 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="O1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>31</v>
       </c>
@@ -1175,50 +1293,53 @@
       <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="J2" t="s">
-        <v>103</v>
+      <c r="H2" t="s">
+        <v>228</v>
       </c>
       <c r="K2" t="s">
-        <v>228</v>
+        <v>101</v>
       </c>
       <c r="L2" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="M2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P2" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" t="s">
         <v>116</v>
       </c>
-      <c r="Q2" t="s">
-        <v>118</v>
-      </c>
-      <c r="R2" t="s">
-        <v>118</v>
-      </c>
       <c r="S2" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="T2" t="s">
-        <v>178</v>
-      </c>
-      <c r="U2">
+        <v>143</v>
+      </c>
+      <c r="U2" t="s">
+        <v>176</v>
+      </c>
+      <c r="V2">
         <v>-44</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>-42</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>-21</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1237,50 +1358,53 @@
       <c r="G3" t="s">
         <v>50</v>
       </c>
-      <c r="J3" t="s">
-        <v>103</v>
+      <c r="H3" t="s">
+        <v>229</v>
       </c>
       <c r="K3" t="s">
-        <v>228</v>
+        <v>101</v>
       </c>
       <c r="L3" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="M3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="N3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="Q3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="R3" t="s">
+        <v>118</v>
+      </c>
+      <c r="S3" t="s">
         <v>21</v>
       </c>
-      <c r="S3" t="s">
-        <v>147</v>
-      </c>
       <c r="T3" t="s">
-        <v>180</v>
-      </c>
-      <c r="U3">
+        <v>145</v>
+      </c>
+      <c r="U3" t="s">
+        <v>178</v>
+      </c>
+      <c r="V3">
         <v>-48</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>-55</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>-15</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1299,50 +1423,53 @@
       <c r="G4" t="s">
         <v>49</v>
       </c>
-      <c r="J4" t="s">
-        <v>103</v>
+      <c r="H4" t="s">
+        <v>230</v>
       </c>
       <c r="K4" t="s">
-        <v>228</v>
+        <v>101</v>
       </c>
       <c r="L4" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="M4" t="s">
+        <v>105</v>
+      </c>
+      <c r="N4" t="s">
+        <v>108</v>
+      </c>
+      <c r="O4" t="s">
+        <v>109</v>
+      </c>
+      <c r="P4" t="s">
         <v>110</v>
       </c>
-      <c r="N4" t="s">
-        <v>111</v>
-      </c>
-      <c r="O4" t="s">
-        <v>112</v>
-      </c>
-      <c r="P4" t="s">
-        <v>116</v>
-      </c>
       <c r="Q4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="R4" t="s">
+        <v>117</v>
+      </c>
+      <c r="S4" t="s">
         <v>21</v>
       </c>
-      <c r="S4" t="s">
-        <v>146</v>
-      </c>
       <c r="T4" t="s">
-        <v>179</v>
-      </c>
-      <c r="U4">
+        <v>144</v>
+      </c>
+      <c r="U4" t="s">
+        <v>177</v>
+      </c>
+      <c r="V4">
         <v>-54</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>-62</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1359,58 +1486,61 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>92</v>
+        <v>231</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="K5" t="s">
-        <v>228</v>
+        <v>101</v>
       </c>
       <c r="L5" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="M5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="N5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="Q5" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="R5" t="s">
+        <v>138</v>
+      </c>
+      <c r="S5" t="s">
         <v>23</v>
       </c>
-      <c r="S5" t="s">
-        <v>167</v>
-      </c>
       <c r="T5" t="s">
-        <v>200</v>
-      </c>
-      <c r="U5">
+        <v>165</v>
+      </c>
+      <c r="U5" t="s">
+        <v>198</v>
+      </c>
+      <c r="V5">
         <v>-46</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>-68</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>14</v>
       </c>
@@ -1429,47 +1559,50 @@
       <c r="G6" t="s">
         <v>60</v>
       </c>
-      <c r="J6" t="s">
-        <v>106</v>
-      </c>
-      <c r="L6" t="s">
-        <v>107</v>
+      <c r="H6" t="s">
+        <v>233</v>
+      </c>
+      <c r="K6" t="s">
+        <v>104</v>
       </c>
       <c r="M6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="N6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="Q6" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="R6" t="s">
+        <v>130</v>
+      </c>
+      <c r="S6" t="s">
         <v>28</v>
       </c>
-      <c r="S6" t="s">
-        <v>159</v>
-      </c>
       <c r="T6" t="s">
-        <v>192</v>
-      </c>
-      <c r="U6">
+        <v>157</v>
+      </c>
+      <c r="U6" t="s">
+        <v>190</v>
+      </c>
+      <c r="V6">
         <v>-27</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>-70</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>34</v>
       </c>
@@ -1492,49 +1625,52 @@
         <v>37</v>
       </c>
       <c r="H7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J7" t="s">
-        <v>105</v>
-      </c>
-      <c r="L7" t="s">
-        <v>107</v>
+        <v>234</v>
+      </c>
+      <c r="I7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" t="s">
+        <v>103</v>
       </c>
       <c r="M7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q7" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="R7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="S7" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="T7" t="s">
-        <v>196</v>
-      </c>
-      <c r="U7">
+        <v>161</v>
+      </c>
+      <c r="U7" t="s">
+        <v>194</v>
+      </c>
+      <c r="V7">
         <v>-53</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>-31</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>33</v>
       </c>
@@ -1557,49 +1693,52 @@
         <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" t="s">
-        <v>106</v>
-      </c>
-      <c r="L8" t="s">
-        <v>107</v>
+        <v>232</v>
+      </c>
+      <c r="I8" t="s">
+        <v>86</v>
+      </c>
+      <c r="K8" t="s">
+        <v>104</v>
       </c>
       <c r="M8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="Q8" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="R8" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="S8" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="T8" t="s">
-        <v>191</v>
-      </c>
-      <c r="U8">
+        <v>156</v>
+      </c>
+      <c r="U8" t="s">
+        <v>189</v>
+      </c>
+      <c r="V8">
         <v>-24</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>-64</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>23</v>
       </c>
@@ -1619,49 +1758,52 @@
         <v>53</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" t="s">
-        <v>105</v>
-      </c>
-      <c r="L9" t="s">
+        <v>235</v>
+      </c>
+      <c r="I9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9" t="s">
+        <v>103</v>
+      </c>
+      <c r="M9" t="s">
+        <v>105</v>
+      </c>
+      <c r="N9" t="s">
         <v>107</v>
       </c>
-      <c r="M9" t="s">
-        <v>109</v>
-      </c>
-      <c r="N9" t="s">
-        <v>113</v>
-      </c>
       <c r="O9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q9" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="R9" t="s">
+        <v>121</v>
+      </c>
+      <c r="S9" t="s">
         <v>24</v>
       </c>
-      <c r="S9" t="s">
-        <v>150</v>
-      </c>
       <c r="T9" t="s">
-        <v>183</v>
-      </c>
-      <c r="U9">
+        <v>148</v>
+      </c>
+      <c r="U9" t="s">
+        <v>181</v>
+      </c>
+      <c r="V9">
         <v>-43</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>-30</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>36</v>
       </c>
@@ -1681,49 +1823,52 @@
         <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" t="s">
-        <v>106</v>
-      </c>
-      <c r="L10" t="s">
-        <v>107</v>
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>236</v>
+      </c>
+      <c r="K10" t="s">
+        <v>104</v>
       </c>
       <c r="M10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="P10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="Q10" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="R10" t="s">
         <v>136</v>
       </c>
       <c r="S10" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="T10" t="s">
-        <v>198</v>
-      </c>
-      <c r="U10">
+        <v>163</v>
+      </c>
+      <c r="U10" t="s">
+        <v>196</v>
+      </c>
+      <c r="V10">
         <v>-33</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>-46</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>33</v>
       </c>
@@ -1745,47 +1890,50 @@
       <c r="G11" t="s">
         <v>59</v>
       </c>
-      <c r="J11" t="s">
-        <v>106</v>
-      </c>
-      <c r="L11" t="s">
-        <v>107</v>
+      <c r="H11" t="s">
+        <v>237</v>
+      </c>
+      <c r="K11" t="s">
+        <v>104</v>
       </c>
       <c r="M11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="Q11" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="R11" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="S11" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="T11" t="s">
-        <v>190</v>
-      </c>
-      <c r="U11">
+        <v>155</v>
+      </c>
+      <c r="U11" t="s">
+        <v>188</v>
+      </c>
+      <c r="V11">
         <v>-28</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>-58</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>25</v>
       </c>
@@ -1805,49 +1953,52 @@
         <v>54</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J12" t="s">
-        <v>105</v>
-      </c>
-      <c r="L12" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" t="s">
+        <v>103</v>
+      </c>
+      <c r="M12" t="s">
+        <v>105</v>
+      </c>
+      <c r="N12" t="s">
         <v>107</v>
       </c>
-      <c r="M12" t="s">
-        <v>109</v>
-      </c>
-      <c r="N12" t="s">
-        <v>113</v>
-      </c>
       <c r="O12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q12" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="R12" t="s">
+        <v>122</v>
+      </c>
+      <c r="S12" t="s">
         <v>26</v>
       </c>
-      <c r="S12" t="s">
-        <v>151</v>
-      </c>
       <c r="T12" t="s">
-        <v>184</v>
-      </c>
-      <c r="U12">
+        <v>149</v>
+      </c>
+      <c r="U12" t="s">
+        <v>182</v>
+      </c>
+      <c r="V12">
         <v>-36</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>-37</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>25</v>
       </c>
@@ -1864,52 +2015,55 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>86</v>
-      </c>
-      <c r="J13" t="s">
-        <v>106</v>
-      </c>
-      <c r="L13" t="s">
+        <v>239</v>
+      </c>
+      <c r="I13" t="s">
+        <v>85</v>
+      </c>
+      <c r="K13" t="s">
+        <v>104</v>
+      </c>
+      <c r="M13" t="s">
+        <v>105</v>
+      </c>
+      <c r="N13" t="s">
         <v>107</v>
       </c>
-      <c r="M13" t="s">
+      <c r="O13" t="s">
         <v>109</v>
       </c>
-      <c r="N13" t="s">
-        <v>111</v>
-      </c>
-      <c r="O13" t="s">
-        <v>111</v>
-      </c>
       <c r="P13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="Q13" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="R13" t="s">
+        <v>137</v>
+      </c>
+      <c r="S13" t="s">
         <v>26</v>
       </c>
-      <c r="S13" t="s">
-        <v>166</v>
-      </c>
       <c r="T13" t="s">
-        <v>199</v>
-      </c>
-      <c r="U13">
+        <v>164</v>
+      </c>
+      <c r="U13" t="s">
+        <v>197</v>
+      </c>
+      <c r="V13">
         <v>-35</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>-50</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>37</v>
       </c>
@@ -1932,49 +2086,52 @@
         <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>89</v>
-      </c>
-      <c r="J14" t="s">
-        <v>106</v>
-      </c>
-      <c r="L14" t="s">
-        <v>107</v>
+        <v>240</v>
+      </c>
+      <c r="I14" t="s">
+        <v>87</v>
+      </c>
+      <c r="K14" t="s">
+        <v>104</v>
       </c>
       <c r="M14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N14" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P14" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="Q14" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="R14" t="s">
         <v>131</v>
       </c>
       <c r="S14" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="T14" t="s">
-        <v>193</v>
-      </c>
-      <c r="U14">
+        <v>158</v>
+      </c>
+      <c r="U14" t="s">
+        <v>191</v>
+      </c>
+      <c r="V14">
         <v>-15</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>-69</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>37</v>
       </c>
@@ -1997,49 +2154,52 @@
         <v>58</v>
       </c>
       <c r="H15" t="s">
-        <v>86</v>
-      </c>
-      <c r="J15" t="s">
-        <v>106</v>
-      </c>
-      <c r="L15" t="s">
-        <v>107</v>
+        <v>241</v>
+      </c>
+      <c r="I15" t="s">
+        <v>85</v>
+      </c>
+      <c r="K15" t="s">
+        <v>104</v>
       </c>
       <c r="M15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N15" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P15" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="Q15" t="s">
+        <v>114</v>
+      </c>
+      <c r="R15" t="s">
+        <v>127</v>
+      </c>
+      <c r="S15" t="s">
         <v>129</v>
       </c>
-      <c r="R15" t="s">
-        <v>131</v>
-      </c>
-      <c r="S15" t="s">
-        <v>156</v>
-      </c>
       <c r="T15" t="s">
-        <v>189</v>
-      </c>
-      <c r="U15">
+        <v>154</v>
+      </c>
+      <c r="U15" t="s">
+        <v>187</v>
+      </c>
+      <c r="V15">
         <v>-27</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>-58</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>39</v>
       </c>
@@ -2061,47 +2221,50 @@
       <c r="G16" t="s">
         <v>61</v>
       </c>
-      <c r="J16" t="s">
-        <v>105</v>
-      </c>
-      <c r="L16" t="s">
-        <v>107</v>
+      <c r="H16" t="s">
+        <v>242</v>
+      </c>
+      <c r="K16" t="s">
+        <v>103</v>
       </c>
       <c r="M16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N16" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P16" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q16" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="R16" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="S16" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="T16" t="s">
-        <v>194</v>
-      </c>
-      <c r="U16">
+        <v>159</v>
+      </c>
+      <c r="U16" t="s">
+        <v>192</v>
+      </c>
+      <c r="V16">
         <v>-7</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>-57</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>25</v>
       </c>
@@ -2121,49 +2284,52 @@
         <v>52</v>
       </c>
       <c r="H17" t="s">
-        <v>86</v>
-      </c>
-      <c r="J17" t="s">
-        <v>105</v>
-      </c>
-      <c r="L17" t="s">
+        <v>243</v>
+      </c>
+      <c r="I17" t="s">
+        <v>85</v>
+      </c>
+      <c r="K17" t="s">
+        <v>103</v>
+      </c>
+      <c r="M17" t="s">
+        <v>105</v>
+      </c>
+      <c r="N17" t="s">
         <v>107</v>
       </c>
-      <c r="M17" t="s">
-        <v>109</v>
-      </c>
-      <c r="N17" t="s">
-        <v>113</v>
-      </c>
       <c r="O17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P17" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q17" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="R17" t="s">
+        <v>120</v>
+      </c>
+      <c r="S17" t="s">
         <v>26</v>
       </c>
-      <c r="S17" t="s">
-        <v>149</v>
-      </c>
       <c r="T17" t="s">
-        <v>182</v>
-      </c>
-      <c r="U17">
+        <v>147</v>
+      </c>
+      <c r="U17" t="s">
+        <v>180</v>
+      </c>
+      <c r="V17">
         <v>-20</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>-54</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>21</v>
       </c>
@@ -2182,47 +2348,50 @@
       <c r="G18" t="s">
         <v>56</v>
       </c>
-      <c r="J18" t="s">
-        <v>104</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="H18" t="s">
+        <v>244</v>
+      </c>
+      <c r="K18" t="s">
+        <v>102</v>
+      </c>
+      <c r="M18" t="s">
+        <v>105</v>
+      </c>
+      <c r="N18" t="s">
         <v>107</v>
       </c>
-      <c r="M18" t="s">
-        <v>109</v>
-      </c>
-      <c r="N18" t="s">
-        <v>113</v>
-      </c>
       <c r="O18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P18" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q18" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="R18" t="s">
+        <v>125</v>
+      </c>
+      <c r="S18" t="s">
         <v>22</v>
       </c>
-      <c r="S18" t="s">
-        <v>154</v>
-      </c>
       <c r="T18" t="s">
-        <v>187</v>
-      </c>
-      <c r="U18">
+        <v>152</v>
+      </c>
+      <c r="U18" t="s">
+        <v>185</v>
+      </c>
+      <c r="V18">
         <v>-40</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>-4</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>41</v>
       </c>
@@ -2244,47 +2413,50 @@
       <c r="G19" t="s">
         <v>55</v>
       </c>
-      <c r="J19" t="s">
-        <v>104</v>
-      </c>
-      <c r="L19" t="s">
-        <v>107</v>
+      <c r="H19" t="s">
+        <v>245</v>
+      </c>
+      <c r="K19" t="s">
+        <v>102</v>
       </c>
       <c r="M19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N19" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P19" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q19" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="R19" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="S19" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="T19" t="s">
-        <v>186</v>
-      </c>
-      <c r="U19">
+        <v>151</v>
+      </c>
+      <c r="U19" t="s">
+        <v>184</v>
+      </c>
+      <c r="V19">
         <v>-26</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>-2</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>41</v>
       </c>
@@ -2306,47 +2478,50 @@
       <c r="G20" t="s">
         <v>57</v>
       </c>
-      <c r="J20" t="s">
-        <v>104</v>
-      </c>
-      <c r="L20" t="s">
-        <v>107</v>
+      <c r="H20" t="s">
+        <v>246</v>
+      </c>
+      <c r="K20" t="s">
+        <v>102</v>
       </c>
       <c r="M20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N20" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q20" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="R20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S20" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="T20" t="s">
-        <v>188</v>
-      </c>
-      <c r="U20">
+        <v>153</v>
+      </c>
+      <c r="U20" t="s">
+        <v>186</v>
+      </c>
+      <c r="V20">
         <v>-30</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>-9</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>28</v>
       </c>
@@ -2366,49 +2541,52 @@
         <v>51</v>
       </c>
       <c r="H21" t="s">
-        <v>86</v>
-      </c>
-      <c r="J21" t="s">
-        <v>104</v>
-      </c>
-      <c r="L21" t="s">
+        <v>247</v>
+      </c>
+      <c r="I21" t="s">
+        <v>85</v>
+      </c>
+      <c r="K21" t="s">
+        <v>102</v>
+      </c>
+      <c r="M21" t="s">
+        <v>105</v>
+      </c>
+      <c r="N21" t="s">
         <v>107</v>
       </c>
-      <c r="M21" t="s">
-        <v>109</v>
-      </c>
-      <c r="N21" t="s">
-        <v>113</v>
-      </c>
       <c r="O21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P21" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="Q21" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="R21" t="s">
+        <v>119</v>
+      </c>
+      <c r="S21" t="s">
         <v>28</v>
       </c>
-      <c r="S21" t="s">
-        <v>148</v>
-      </c>
       <c r="T21" t="s">
-        <v>181</v>
-      </c>
-      <c r="U21">
+        <v>146</v>
+      </c>
+      <c r="U21" t="s">
+        <v>179</v>
+      </c>
+      <c r="V21">
         <v>-21</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>3</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>43</v>
       </c>
@@ -2428,52 +2606,55 @@
         <v>32</v>
       </c>
       <c r="G22" t="s">
-        <v>32</v>
+        <v>264</v>
       </c>
       <c r="H22" t="s">
-        <v>87</v>
-      </c>
-      <c r="J22" t="s">
-        <v>104</v>
-      </c>
-      <c r="L22" t="s">
-        <v>107</v>
+        <v>266</v>
+      </c>
+      <c r="I22" t="s">
+        <v>263</v>
+      </c>
+      <c r="K22" t="s">
+        <v>102</v>
       </c>
       <c r="M22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N22" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P22" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="Q22" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="R22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S22" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="T22" t="s">
-        <v>185</v>
-      </c>
-      <c r="U22">
+        <v>150</v>
+      </c>
+      <c r="U22" t="s">
+        <v>183</v>
+      </c>
+      <c r="V22">
         <v>-48</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>6</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2490,49 +2671,55 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J23" t="s">
-        <v>104</v>
-      </c>
-      <c r="L23" t="s">
+        <v>262</v>
+      </c>
+      <c r="H23" t="s">
+        <v>265</v>
+      </c>
+      <c r="I23" t="s">
+        <v>261</v>
+      </c>
+      <c r="K23" t="s">
+        <v>102</v>
+      </c>
+      <c r="M23" t="s">
+        <v>105</v>
+      </c>
+      <c r="N23" t="s">
         <v>107</v>
       </c>
-      <c r="M23" t="s">
-        <v>109</v>
-      </c>
-      <c r="N23" t="s">
-        <v>113</v>
-      </c>
       <c r="O23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P23" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q23" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="R23" t="s">
+        <v>135</v>
+      </c>
+      <c r="S23" t="s">
         <v>22</v>
       </c>
-      <c r="S23" t="s">
-        <v>164</v>
-      </c>
       <c r="T23" t="s">
-        <v>197</v>
-      </c>
-      <c r="U23">
+        <v>162</v>
+      </c>
+      <c r="U23" t="s">
+        <v>195</v>
+      </c>
+      <c r="V23">
         <v>-49</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>1</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>39</v>
       </c>
@@ -2555,49 +2742,52 @@
         <v>62</v>
       </c>
       <c r="H24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J24" t="s">
-        <v>105</v>
-      </c>
-      <c r="L24" t="s">
-        <v>108</v>
+        <v>248</v>
+      </c>
+      <c r="I24" t="s">
+        <v>88</v>
+      </c>
+      <c r="K24" t="s">
+        <v>103</v>
       </c>
       <c r="M24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N24" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P24" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q24" t="s">
         <v>114</v>
       </c>
-      <c r="P24" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>135</v>
-      </c>
       <c r="R24" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="S24" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="T24" t="s">
-        <v>195</v>
-      </c>
-      <c r="U24">
+        <v>160</v>
+      </c>
+      <c r="U24" t="s">
+        <v>193</v>
+      </c>
+      <c r="V24">
         <v>-4</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>-62</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>147</v>
       </c>
@@ -2617,52 +2807,55 @@
         <v>43</v>
       </c>
       <c r="G25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H25" t="s">
-        <v>97</v>
-      </c>
-      <c r="J25" t="s">
-        <v>104</v>
-      </c>
-      <c r="L25" t="s">
-        <v>109</v>
+        <v>265</v>
+      </c>
+      <c r="I25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K25" t="s">
+        <v>102</v>
       </c>
       <c r="M25" t="s">
         <v>107</v>
       </c>
       <c r="N25" t="s">
+        <v>105</v>
+      </c>
+      <c r="O25" t="s">
+        <v>111</v>
+      </c>
+      <c r="P25" t="s">
         <v>113</v>
       </c>
-      <c r="O25" t="s">
+      <c r="Q25" t="s">
         <v>115</v>
       </c>
-      <c r="P25" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>29</v>
       </c>
-      <c r="R25" t="s">
-        <v>125</v>
-      </c>
       <c r="S25" t="s">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="T25" t="s">
-        <v>210</v>
-      </c>
-      <c r="U25">
+        <v>168</v>
+      </c>
+      <c r="U25" t="s">
+        <v>208</v>
+      </c>
+      <c r="V25">
         <v>59</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>6</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>101</v>
       </c>
@@ -2681,50 +2874,53 @@
       <c r="G26" t="s">
         <v>40</v>
       </c>
-      <c r="J26" t="s">
-        <v>103</v>
+      <c r="H26" t="s">
+        <v>249</v>
       </c>
       <c r="K26" t="s">
-        <v>228</v>
+        <v>101</v>
       </c>
       <c r="L26" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="M26" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="N26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P26" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="Q26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="R26" t="s">
+        <v>116</v>
+      </c>
+      <c r="S26" t="s">
         <v>20</v>
       </c>
-      <c r="S26" t="s">
-        <v>168</v>
-      </c>
       <c r="T26" t="s">
-        <v>201</v>
-      </c>
-      <c r="U26">
+        <v>166</v>
+      </c>
+      <c r="U26" t="s">
+        <v>199</v>
+      </c>
+      <c r="V26">
         <v>48</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>-51</v>
       </c>
-      <c r="W26">
+      <c r="X26">
         <v>-17</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>135</v>
       </c>
@@ -2744,55 +2940,58 @@
         <v>40</v>
       </c>
       <c r="G27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H27" t="s">
-        <v>93</v>
-      </c>
-      <c r="J27" t="s">
-        <v>103</v>
+        <v>250</v>
+      </c>
+      <c r="I27" t="s">
+        <v>91</v>
       </c>
       <c r="K27" t="s">
-        <v>228</v>
+        <v>101</v>
       </c>
       <c r="L27" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="M27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N27" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P27" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q27" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="R27" t="s">
         <v>118</v>
       </c>
       <c r="S27" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="T27" t="s">
-        <v>203</v>
-      </c>
-      <c r="U27">
+        <v>143</v>
+      </c>
+      <c r="U27" t="s">
+        <v>201</v>
+      </c>
+      <c r="V27">
         <v>58</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>-56</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>136</v>
       </c>
@@ -2812,52 +3011,55 @@
         <v>39</v>
       </c>
       <c r="G28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J28" t="s">
-        <v>103</v>
+        <v>66</v>
+      </c>
+      <c r="H28" t="s">
+        <v>251</v>
       </c>
       <c r="K28" t="s">
-        <v>228</v>
+        <v>101</v>
       </c>
       <c r="L28" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="M28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N28" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P28" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>115</v>
+      </c>
+      <c r="R28" t="s">
         <v>117</v>
       </c>
-      <c r="Q28" t="s">
-        <v>119</v>
-      </c>
-      <c r="R28" t="s">
-        <v>120</v>
-      </c>
       <c r="S28" t="s">
-        <v>169</v>
+        <v>118</v>
       </c>
       <c r="T28" t="s">
-        <v>202</v>
-      </c>
-      <c r="U28">
+        <v>167</v>
+      </c>
+      <c r="U28" t="s">
+        <v>200</v>
+      </c>
+      <c r="V28">
         <v>52</v>
       </c>
-      <c r="V28">
+      <c r="W28">
         <v>-57</v>
       </c>
-      <c r="W28">
+      <c r="X28">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>115</v>
       </c>
@@ -2874,55 +3076,58 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H29" t="s">
-        <v>98</v>
+        <v>233</v>
       </c>
       <c r="I29" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J29" t="s">
-        <v>106</v>
-      </c>
-      <c r="L29" t="s">
-        <v>107</v>
+        <v>100</v>
+      </c>
+      <c r="K29" t="s">
+        <v>104</v>
       </c>
       <c r="M29" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="N29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P29" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="Q29" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="R29" t="s">
+        <v>130</v>
+      </c>
+      <c r="S29" t="s">
         <v>29</v>
       </c>
-      <c r="S29" t="s">
-        <v>172</v>
-      </c>
       <c r="T29" t="s">
-        <v>215</v>
-      </c>
-      <c r="U29">
+        <v>170</v>
+      </c>
+      <c r="U29" t="s">
+        <v>213</v>
+      </c>
+      <c r="V29">
         <v>31</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>-67</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>137</v>
       </c>
@@ -2944,47 +3149,50 @@
       <c r="G30" t="s">
         <v>47</v>
       </c>
-      <c r="J30" t="s">
-        <v>105</v>
-      </c>
-      <c r="L30" t="s">
-        <v>107</v>
+      <c r="H30" t="s">
+        <v>234</v>
+      </c>
+      <c r="K30" t="s">
+        <v>103</v>
       </c>
       <c r="M30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N30" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P30" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>115</v>
+      </c>
+      <c r="R30" t="s">
+        <v>134</v>
+      </c>
+      <c r="S30" t="s">
         <v>117</v>
       </c>
-      <c r="Q30" t="s">
-        <v>136</v>
-      </c>
-      <c r="R30" t="s">
-        <v>119</v>
-      </c>
-      <c r="S30" t="s">
-        <v>176</v>
-      </c>
       <c r="T30" t="s">
-        <v>222</v>
-      </c>
-      <c r="U30">
+        <v>174</v>
+      </c>
+      <c r="U30" t="s">
+        <v>220</v>
+      </c>
+      <c r="V30">
         <v>55</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>-25</v>
       </c>
-      <c r="W30">
+      <c r="X30">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>114</v>
       </c>
@@ -3001,49 +3209,52 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>81</v>
-      </c>
-      <c r="J31" t="s">
-        <v>106</v>
-      </c>
-      <c r="L31" t="s">
-        <v>107</v>
+        <v>80</v>
+      </c>
+      <c r="H31" t="s">
+        <v>252</v>
+      </c>
+      <c r="K31" t="s">
+        <v>104</v>
       </c>
       <c r="M31" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="N31" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P31" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="Q31" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="R31" t="s">
+        <v>129</v>
+      </c>
+      <c r="S31" t="s">
         <v>28</v>
       </c>
-      <c r="S31" t="s">
-        <v>158</v>
-      </c>
       <c r="T31" t="s">
-        <v>218</v>
-      </c>
-      <c r="U31">
+        <v>156</v>
+      </c>
+      <c r="U31" t="s">
+        <v>216</v>
+      </c>
+      <c r="V31">
         <v>17</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <v>-76</v>
       </c>
-      <c r="W31">
+      <c r="X31">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>138</v>
       </c>
@@ -3063,49 +3274,52 @@
         <v>42</v>
       </c>
       <c r="G32" t="s">
-        <v>73</v>
-      </c>
-      <c r="J32" t="s">
-        <v>105</v>
-      </c>
-      <c r="L32" t="s">
-        <v>107</v>
+        <v>72</v>
+      </c>
+      <c r="H32" t="s">
+        <v>238</v>
+      </c>
+      <c r="K32" t="s">
+        <v>103</v>
       </c>
       <c r="M32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N32" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P32" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q32" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="R32" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="S32" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="T32" t="s">
-        <v>209</v>
-      </c>
-      <c r="U32">
+        <v>161</v>
+      </c>
+      <c r="U32" t="s">
+        <v>207</v>
+      </c>
+      <c r="V32">
         <v>38</v>
       </c>
-      <c r="V32">
+      <c r="W32">
         <v>-39</v>
       </c>
-      <c r="W32">
+      <c r="X32">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>124</v>
       </c>
@@ -3122,49 +3336,52 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>72</v>
-      </c>
-      <c r="J33" t="s">
-        <v>105</v>
-      </c>
-      <c r="L33" t="s">
+        <v>71</v>
+      </c>
+      <c r="H33" t="s">
+        <v>235</v>
+      </c>
+      <c r="K33" t="s">
+        <v>103</v>
+      </c>
+      <c r="M33" t="s">
+        <v>105</v>
+      </c>
+      <c r="N33" t="s">
         <v>107</v>
       </c>
-      <c r="M33" t="s">
-        <v>109</v>
-      </c>
-      <c r="N33" t="s">
-        <v>113</v>
-      </c>
       <c r="O33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P33" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q33" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="R33" t="s">
+        <v>136</v>
+      </c>
+      <c r="S33" t="s">
         <v>24</v>
       </c>
-      <c r="S33" t="s">
-        <v>150</v>
-      </c>
       <c r="T33" t="s">
-        <v>208</v>
-      </c>
-      <c r="U33">
+        <v>148</v>
+      </c>
+      <c r="U33" t="s">
+        <v>206</v>
+      </c>
+      <c r="V33">
         <v>43</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <v>-29</v>
       </c>
-      <c r="W33">
+      <c r="X33">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>142</v>
       </c>
@@ -3184,49 +3401,52 @@
         <v>44</v>
       </c>
       <c r="G34" t="s">
-        <v>79</v>
-      </c>
-      <c r="J34" t="s">
-        <v>106</v>
-      </c>
-      <c r="L34" t="s">
-        <v>107</v>
+        <v>78</v>
+      </c>
+      <c r="H34" t="s">
+        <v>253</v>
+      </c>
+      <c r="K34" t="s">
+        <v>104</v>
       </c>
       <c r="M34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N34" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P34" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="Q34" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="R34" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="S34" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="T34" t="s">
-        <v>216</v>
-      </c>
-      <c r="U34">
+        <v>155</v>
+      </c>
+      <c r="U34" t="s">
+        <v>214</v>
+      </c>
+      <c r="V34">
         <v>28</v>
       </c>
-      <c r="V34">
+      <c r="W34">
         <v>-61</v>
       </c>
-      <c r="W34">
+      <c r="X34">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>138</v>
       </c>
@@ -3246,49 +3466,52 @@
         <v>42</v>
       </c>
       <c r="G35" t="s">
-        <v>84</v>
-      </c>
-      <c r="J35" t="s">
-        <v>106</v>
-      </c>
-      <c r="L35" t="s">
-        <v>107</v>
+        <v>83</v>
+      </c>
+      <c r="H35" t="s">
+        <v>236</v>
+      </c>
+      <c r="K35" t="s">
+        <v>104</v>
       </c>
       <c r="M35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N35" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O35" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="P35" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="Q35" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="R35" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="S35" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
       <c r="T35" t="s">
-        <v>223</v>
-      </c>
-      <c r="U35">
+        <v>175</v>
+      </c>
+      <c r="U35" t="s">
+        <v>221</v>
+      </c>
+      <c r="V35">
         <v>32</v>
       </c>
-      <c r="V35">
+      <c r="W35">
         <v>-46</v>
       </c>
-      <c r="W35">
+      <c r="X35">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>115</v>
       </c>
@@ -3305,49 +3528,52 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>80</v>
-      </c>
-      <c r="J36" t="s">
-        <v>106</v>
-      </c>
-      <c r="L36" t="s">
-        <v>107</v>
+        <v>79</v>
+      </c>
+      <c r="H36" t="s">
+        <v>254</v>
+      </c>
+      <c r="K36" t="s">
+        <v>104</v>
       </c>
       <c r="M36" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="N36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P36" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="Q36" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="R36" t="s">
+        <v>137</v>
+      </c>
+      <c r="S36" t="s">
         <v>29</v>
       </c>
-      <c r="S36" t="s">
-        <v>166</v>
-      </c>
       <c r="T36" t="s">
-        <v>217</v>
-      </c>
-      <c r="U36">
+        <v>164</v>
+      </c>
+      <c r="U36" t="s">
+        <v>215</v>
+      </c>
+      <c r="V36">
         <v>20</v>
       </c>
-      <c r="V36">
+      <c r="W36">
         <v>-68</v>
       </c>
-      <c r="W36">
+      <c r="X36">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>124</v>
       </c>
@@ -3364,52 +3590,55 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H37" t="s">
-        <v>96</v>
-      </c>
-      <c r="J37" t="s">
-        <v>105</v>
-      </c>
-      <c r="L37" t="s">
+        <v>255</v>
+      </c>
+      <c r="I37" t="s">
+        <v>94</v>
+      </c>
+      <c r="K37" t="s">
+        <v>103</v>
+      </c>
+      <c r="M37" t="s">
+        <v>105</v>
+      </c>
+      <c r="N37" t="s">
         <v>107</v>
       </c>
-      <c r="M37" t="s">
-        <v>109</v>
-      </c>
-      <c r="N37" t="s">
-        <v>113</v>
-      </c>
       <c r="O37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P37" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q37" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="R37" t="s">
+        <v>131</v>
+      </c>
+      <c r="S37" t="s">
         <v>24</v>
       </c>
-      <c r="S37" t="s">
-        <v>151</v>
-      </c>
       <c r="T37" t="s">
-        <v>207</v>
-      </c>
-      <c r="U37">
+        <v>149</v>
+      </c>
+      <c r="U37" t="s">
+        <v>205</v>
+      </c>
+      <c r="V37">
         <v>38</v>
       </c>
-      <c r="V37">
+      <c r="W37">
         <v>-38</v>
       </c>
-      <c r="W37">
+      <c r="X37">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>128</v>
       </c>
@@ -3426,49 +3655,52 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>85</v>
-      </c>
-      <c r="J38" t="s">
-        <v>106</v>
-      </c>
-      <c r="L38" t="s">
+        <v>84</v>
+      </c>
+      <c r="H38" t="s">
+        <v>239</v>
+      </c>
+      <c r="K38" t="s">
+        <v>104</v>
+      </c>
+      <c r="M38" t="s">
+        <v>105</v>
+      </c>
+      <c r="N38" t="s">
         <v>107</v>
       </c>
-      <c r="M38" t="s">
+      <c r="O38" t="s">
         <v>109</v>
       </c>
-      <c r="N38" t="s">
-        <v>111</v>
-      </c>
-      <c r="O38" t="s">
-        <v>111</v>
-      </c>
       <c r="P38" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="Q38" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="R38" t="s">
+        <v>127</v>
+      </c>
+      <c r="S38" t="s">
         <v>27</v>
       </c>
-      <c r="S38" t="s">
-        <v>160</v>
-      </c>
       <c r="T38" t="s">
-        <v>224</v>
-      </c>
-      <c r="U38">
+        <v>158</v>
+      </c>
+      <c r="U38" t="s">
+        <v>222</v>
+      </c>
+      <c r="V38">
         <v>33</v>
       </c>
-      <c r="V38">
+      <c r="W38">
         <v>-52</v>
       </c>
-      <c r="W38">
+      <c r="X38">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>140</v>
       </c>
@@ -3488,49 +3720,52 @@
         <v>45</v>
       </c>
       <c r="G39" t="s">
-        <v>82</v>
-      </c>
-      <c r="J39" t="s">
-        <v>106</v>
-      </c>
-      <c r="L39" t="s">
-        <v>107</v>
+        <v>81</v>
+      </c>
+      <c r="H39" t="s">
+        <v>256</v>
+      </c>
+      <c r="K39" t="s">
+        <v>104</v>
       </c>
       <c r="M39" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N39" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O39" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="P39" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Q39" t="s">
+        <v>115</v>
+      </c>
+      <c r="R39" t="s">
+        <v>132</v>
+      </c>
+      <c r="S39" t="s">
         <v>134</v>
       </c>
-      <c r="R39" t="s">
-        <v>136</v>
-      </c>
-      <c r="S39" t="s">
-        <v>173</v>
-      </c>
       <c r="T39" t="s">
-        <v>219</v>
-      </c>
-      <c r="U39">
+        <v>171</v>
+      </c>
+      <c r="U39" t="s">
+        <v>217</v>
+      </c>
+      <c r="V39">
         <v>7</v>
       </c>
-      <c r="V39">
+      <c r="W39">
         <v>-70</v>
       </c>
-      <c r="W39">
+      <c r="X39">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>142</v>
       </c>
@@ -3550,49 +3785,52 @@
         <v>44</v>
       </c>
       <c r="G40" t="s">
-        <v>77</v>
-      </c>
-      <c r="J40" t="s">
-        <v>106</v>
-      </c>
-      <c r="L40" t="s">
-        <v>107</v>
+        <v>76</v>
+      </c>
+      <c r="H40" t="s">
+        <v>257</v>
+      </c>
+      <c r="K40" t="s">
+        <v>104</v>
       </c>
       <c r="M40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N40" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P40" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="Q40" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="R40" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S40" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="T40" t="s">
-        <v>214</v>
-      </c>
-      <c r="U40">
+        <v>154</v>
+      </c>
+      <c r="U40" t="s">
+        <v>212</v>
+      </c>
+      <c r="V40">
         <v>26</v>
       </c>
-      <c r="V40">
+      <c r="W40">
         <v>-58</v>
       </c>
-      <c r="W40">
+      <c r="X40">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>143</v>
       </c>
@@ -3612,49 +3850,52 @@
         <v>46</v>
       </c>
       <c r="G41" t="s">
-        <v>83</v>
-      </c>
-      <c r="J41" t="s">
-        <v>105</v>
-      </c>
-      <c r="L41" t="s">
-        <v>107</v>
+        <v>82</v>
+      </c>
+      <c r="H41" t="s">
+        <v>258</v>
+      </c>
+      <c r="K41" t="s">
+        <v>103</v>
       </c>
       <c r="M41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N41" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P41" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q41" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="R41" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="S41" t="s">
-        <v>175</v>
+        <v>136</v>
       </c>
       <c r="T41" t="s">
-        <v>221</v>
-      </c>
-      <c r="U41">
+        <v>173</v>
+      </c>
+      <c r="U41" t="s">
+        <v>219</v>
+      </c>
+      <c r="V41">
         <v>7</v>
       </c>
-      <c r="V41">
+      <c r="W41">
         <v>-53</v>
       </c>
-      <c r="W41">
+      <c r="X41">
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>140</v>
       </c>
@@ -3676,47 +3917,50 @@
       <c r="G42" t="s">
         <v>46</v>
       </c>
-      <c r="J42" t="s">
-        <v>106</v>
-      </c>
-      <c r="L42" t="s">
-        <v>107</v>
+      <c r="H42" t="s">
+        <v>259</v>
+      </c>
+      <c r="K42" t="s">
+        <v>104</v>
       </c>
       <c r="M42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N42" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P42" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="Q42" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="R42" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="S42" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="T42" t="s">
-        <v>220</v>
-      </c>
-      <c r="U42">
+        <v>172</v>
+      </c>
+      <c r="U42" t="s">
+        <v>218</v>
+      </c>
+      <c r="V42">
         <v>13</v>
       </c>
-      <c r="V42">
+      <c r="W42">
         <v>-63</v>
       </c>
-      <c r="W42">
+      <c r="X42">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>128</v>
       </c>
@@ -3733,49 +3977,52 @@
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>70</v>
-      </c>
-      <c r="J43" t="s">
-        <v>105</v>
-      </c>
-      <c r="L43" t="s">
+        <v>69</v>
+      </c>
+      <c r="H43" t="s">
+        <v>243</v>
+      </c>
+      <c r="K43" t="s">
+        <v>103</v>
+      </c>
+      <c r="M43" t="s">
+        <v>105</v>
+      </c>
+      <c r="N43" t="s">
         <v>107</v>
       </c>
-      <c r="M43" t="s">
-        <v>109</v>
-      </c>
-      <c r="N43" t="s">
-        <v>113</v>
-      </c>
       <c r="O43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P43" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q43" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="R43" t="s">
+        <v>140</v>
+      </c>
+      <c r="S43" t="s">
         <v>27</v>
       </c>
-      <c r="S43" t="s">
-        <v>161</v>
-      </c>
       <c r="T43" t="s">
-        <v>206</v>
-      </c>
-      <c r="U43">
+        <v>159</v>
+      </c>
+      <c r="U43" t="s">
+        <v>204</v>
+      </c>
+      <c r="V43">
         <v>25</v>
       </c>
-      <c r="V43">
+      <c r="W43">
         <v>-51</v>
       </c>
-      <c r="W43">
+      <c r="X43">
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>125</v>
       </c>
@@ -3792,49 +4039,52 @@
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>76</v>
-      </c>
-      <c r="J44" t="s">
-        <v>104</v>
-      </c>
-      <c r="L44" t="s">
+        <v>75</v>
+      </c>
+      <c r="H44" t="s">
+        <v>244</v>
+      </c>
+      <c r="K44" t="s">
+        <v>102</v>
+      </c>
+      <c r="M44" t="s">
+        <v>105</v>
+      </c>
+      <c r="N44" t="s">
         <v>107</v>
       </c>
-      <c r="M44" t="s">
-        <v>109</v>
-      </c>
-      <c r="N44" t="s">
-        <v>113</v>
-      </c>
       <c r="O44" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P44" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q44" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="R44" t="s">
+        <v>125</v>
+      </c>
+      <c r="S44" t="s">
         <v>25</v>
       </c>
-      <c r="S44" t="s">
-        <v>154</v>
-      </c>
       <c r="T44" t="s">
-        <v>213</v>
-      </c>
-      <c r="U44">
+        <v>152</v>
+      </c>
+      <c r="U44" t="s">
+        <v>211</v>
+      </c>
+      <c r="V44">
         <v>39</v>
       </c>
-      <c r="V44">
+      <c r="W44">
         <v>-3</v>
       </c>
-      <c r="W44">
+      <c r="X44">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>131</v>
       </c>
@@ -3851,49 +4101,52 @@
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>75</v>
-      </c>
-      <c r="J45" t="s">
-        <v>104</v>
-      </c>
-      <c r="L45" t="s">
+        <v>74</v>
+      </c>
+      <c r="H45" t="s">
+        <v>245</v>
+      </c>
+      <c r="K45" t="s">
+        <v>102</v>
+      </c>
+      <c r="M45" t="s">
+        <v>105</v>
+      </c>
+      <c r="N45" t="s">
         <v>107</v>
       </c>
-      <c r="M45" t="s">
-        <v>109</v>
-      </c>
-      <c r="N45" t="s">
-        <v>113</v>
-      </c>
       <c r="O45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P45" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q45" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="R45" t="s">
+        <v>124</v>
+      </c>
+      <c r="S45" t="s">
         <v>30</v>
       </c>
-      <c r="S45" t="s">
-        <v>153</v>
-      </c>
       <c r="T45" t="s">
-        <v>212</v>
-      </c>
-      <c r="U45">
+        <v>151</v>
+      </c>
+      <c r="U45" t="s">
+        <v>210</v>
+      </c>
+      <c r="V45">
         <v>27</v>
       </c>
-      <c r="V45">
+      <c r="W45">
         <v>-4</v>
       </c>
-      <c r="W45">
+      <c r="X45">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>131</v>
       </c>
@@ -3913,52 +4166,55 @@
         <v>41</v>
       </c>
       <c r="H46" t="s">
-        <v>94</v>
+        <v>247</v>
       </c>
       <c r="I46" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="J46" t="s">
-        <v>104</v>
-      </c>
-      <c r="L46" t="s">
+        <v>98</v>
+      </c>
+      <c r="K46" t="s">
+        <v>102</v>
+      </c>
+      <c r="M46" t="s">
+        <v>105</v>
+      </c>
+      <c r="N46" t="s">
         <v>107</v>
       </c>
-      <c r="M46" t="s">
-        <v>109</v>
-      </c>
-      <c r="N46" t="s">
-        <v>113</v>
-      </c>
       <c r="O46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P46" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q46" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="R46" t="s">
+        <v>126</v>
+      </c>
+      <c r="S46" t="s">
         <v>30</v>
       </c>
-      <c r="S46" t="s">
-        <v>155</v>
-      </c>
       <c r="T46" t="s">
-        <v>204</v>
-      </c>
-      <c r="U46">
+        <v>153</v>
+      </c>
+      <c r="U46" t="s">
+        <v>202</v>
+      </c>
+      <c r="V46">
         <v>24</v>
       </c>
-      <c r="V46">
+      <c r="W46">
         <v>-4</v>
       </c>
-      <c r="W46">
+      <c r="X46">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>147</v>
       </c>
@@ -3980,47 +4236,50 @@
       <c r="G47" t="s">
         <v>43</v>
       </c>
-      <c r="J47" t="s">
-        <v>104</v>
-      </c>
-      <c r="L47" t="s">
-        <v>107</v>
+      <c r="H47" t="s">
+        <v>266</v>
+      </c>
+      <c r="K47" t="s">
+        <v>102</v>
       </c>
       <c r="M47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N47" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P47" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="Q47" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="R47" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S47" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="T47" t="s">
-        <v>211</v>
-      </c>
-      <c r="U47">
+        <v>169</v>
+      </c>
+      <c r="U47" t="s">
+        <v>209</v>
+      </c>
+      <c r="V47">
         <v>48</v>
       </c>
-      <c r="V47">
+      <c r="W47">
         <v>8</v>
       </c>
-      <c r="W47">
+      <c r="X47">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>146</v>
       </c>
@@ -4040,56 +4299,59 @@
         <v>41</v>
       </c>
       <c r="G48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H48" t="s">
-        <v>95</v>
+        <v>260</v>
       </c>
       <c r="I48" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="J48" t="s">
-        <v>104</v>
-      </c>
-      <c r="L48" t="s">
-        <v>108</v>
+        <v>99</v>
+      </c>
+      <c r="K48" t="s">
+        <v>102</v>
       </c>
       <c r="M48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N48" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P48" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="Q48" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="R48" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="S48" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="T48" t="s">
-        <v>205</v>
-      </c>
-      <c r="U48">
+        <v>146</v>
+      </c>
+      <c r="U48" t="s">
+        <v>203</v>
+      </c>
+      <c r="V48">
         <v>24</v>
       </c>
-      <c r="V48">
+      <c r="W48">
         <v>8</v>
       </c>
-      <c r="W48">
+      <c r="X48">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W48">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X48">
     <sortCondition ref="B2:B48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>